<commit_message>
atualizando Planilhas/Matheus - Python.xlsx
</commit_message>
<xml_diff>
--- a/Planilhas/Matheus - Python.xlsx
+++ b/Planilhas/Matheus - Python.xlsx
@@ -18,25 +18,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>$/hour</t>
-  </si>
-  <si>
-    <t>Worked Hour</t>
-  </si>
-  <si>
-    <t>Cust</t>
-  </si>
-  <si>
-    <t>Basketball ESPN Parser</t>
-  </si>
-  <si>
-    <t>Baseball ESPN Parser</t>
-  </si>
-  <si>
-    <t>Baseball CBS Parser</t>
+    <t>Valor da Hora</t>
+  </si>
+  <si>
+    <t>Horas Trabalhadas</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Tarefa</t>
+  </si>
+  <si>
+    <t>Parser Basketball ESPN</t>
+  </si>
+  <si>
+    <t>Parser Baseball ESPN</t>
+  </si>
+  <si>
+    <t>Parser Baseball CBS</t>
   </si>
 </sst>
 </file>
@@ -46,7 +46,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-540A]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,15 +69,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,11 +81,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,26 +117,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="20% - Ênfase3" xfId="2" builtinId="38"/>
-    <cellStyle name="Bom" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
@@ -442,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E12"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,121 +446,119 @@
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="26.25" customHeight="1">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="2:6" ht="26.25" customHeight="1">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5">
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>10</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <f>(C2 *D2)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:6">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
         <f t="shared" ref="E3:E10" si="0">PRODUCT(C3,D3)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="E12" s="6">
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
         <f>SUM(E2:E10)</f>
         <v>80</v>
       </c>

</xml_diff>